<commit_message>
Added auth into nodeexpressapi
</commit_message>
<xml_diff>
--- a/Aufgabenbereiche.xlsx
+++ b/Aufgabenbereiche.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael Ulrich\IBS_SS21\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2C5091B3-8932-46B5-BAE5-8B5328BD11BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{941D10AA-6D3F-4C0D-AD93-0255E876ADBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C5CAF5C4-B23E-4FDB-AE4B-12EABFB0B58D}"/>
+    <workbookView xWindow="3270" yWindow="2205" windowWidth="21600" windowHeight="11385" xr2:uid="{C5CAF5C4-B23E-4FDB-AE4B-12EABFB0B58D}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>Aufgaben:</t>
   </si>
@@ -91,6 +91,13 @@
   </si>
   <si>
     <t>Vero</t>
+  </si>
+  <si>
+    <t>#Sicherheitsaspekte : Connectstring, Einloggdaten in .env speichern  #Connectiondaten müssen auf aufgesetze Datenbanken angepasst werden, möglich wär auch lokal
+#Datenschemas erstellen</t>
+  </si>
+  <si>
+    <t>Priorität</t>
   </si>
 </sst>
 </file>
@@ -126,9 +133,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -443,20 +453,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0A68A5C-D9C1-4BB8-9C8C-E2E12C0DD6D5}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="79.85546875" customWidth="1"/>
     <col min="2" max="2" width="23.42578125" customWidth="1"/>
-    <col min="4" max="4" width="40.7109375" customWidth="1"/>
+    <col min="4" max="4" width="60.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -469,28 +479,43 @@
       <c r="D1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -500,8 +525,14 @@
       <c r="C6" s="1">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -514,16 +545,22 @@
       <c r="D7" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
       <c r="B8" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -537,9 +574,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Nicht lauffähige Version. Implementierung der Profiles. Aufgabenbereiche aktuallisiert
</commit_message>
<xml_diff>
--- a/Aufgabenbereiche.xlsx
+++ b/Aufgabenbereiche.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael Ulrich\IBS_SS21\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simon Ruttmann\Desktop\InternetbasierteSystemeProjekt\IBS_SS21\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7B6D008-C27E-4581-849A-EBE47B9FF84B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C5CAF5C4-B23E-4FDB-AE4B-12EABFB0B58D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="58">
   <si>
     <t>Aufgaben:</t>
   </si>
@@ -42,12 +41,6 @@
     <t>Corona-Karte</t>
   </si>
   <si>
-    <t>GUI</t>
-  </si>
-  <si>
-    <t>(React)</t>
-  </si>
-  <si>
     <t>Verantwortlich:</t>
   </si>
   <si>
@@ -66,9 +59,6 @@
     <t>Websockets</t>
   </si>
   <si>
-    <t>Login(cookies)</t>
-  </si>
-  <si>
     <t>Fortschritt</t>
   </si>
   <si>
@@ -87,30 +77,189 @@
     <t>Simon</t>
   </si>
   <si>
-    <t>Copy-Pasted</t>
-  </si>
-  <si>
     <t>Vero</t>
   </si>
   <si>
-    <t>#Sicherheitsaspekte : Connectstring, Einloggdaten in .env speichern  #Connectiondaten müssen auf aufgesetze Datenbanken angepasst werden, möglich wär auch lokal
+    <t>Priorität</t>
+  </si>
+  <si>
+    <t>Fertigstellung(Speziell mit Docker)</t>
+  </si>
+  <si>
+    <t>Registrierung: E-Mail, PW muss auf unique geprüft werden</t>
+  </si>
+  <si>
+    <t>Websockets MySql</t>
+  </si>
+  <si>
+    <t>Websockets MongoDb</t>
+  </si>
+  <si>
+    <t>Websockets Frontend</t>
+  </si>
+  <si>
+    <t>Kann aus Auth. System großteils übernommen werden</t>
+  </si>
+  <si>
+    <t>~65%</t>
+  </si>
+  <si>
+    <t>Cookies</t>
+  </si>
+  <si>
+    <t>Login/Registrierung Frontend</t>
+  </si>
+  <si>
+    <t>Login/Registrierung</t>
+  </si>
+  <si>
+    <t>Authentifizierung &amp; Session</t>
+  </si>
+  <si>
+    <t>~95%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Userverwaltung / Profil </t>
+  </si>
+  <si>
+    <t>~70%</t>
+  </si>
+  <si>
+    <t>Websockets Logik</t>
+  </si>
+  <si>
+    <t>Dummy Implementierung getestet</t>
+  </si>
+  <si>
+    <t>Navigationsmenüs</t>
+  </si>
+  <si>
+    <t>Serverseitig und Clientseitig verfügbar, beidseitig in Verwendung</t>
+  </si>
+  <si>
+    <t>Redirects</t>
+  </si>
+  <si>
+    <t>Authentifiziert: Login-&gt;Index, Register-&gt;Index Unauthentifiziert: Profil -&gt; Anmelden</t>
+  </si>
+  <si>
+    <t>Basic Frontend &amp; Navigation/Redirects</t>
+  </si>
+  <si>
+    <t>Sonntag oder Montag erledigt</t>
+  </si>
+  <si>
+    <t>#Sicherheitsaspekte : Connectstring, Einloggdaten in .env speichern  #Connectiondaten müssen auf aufgesetze Datenbanken angepasst werden, möglich wär auch lokal ? Möglich? Mit Docker läufts lokal...
 #Datenschemas erstellen</t>
   </si>
   <si>
-    <t>Priorität</t>
-  </si>
-  <si>
-    <t>Fertigstellung(Speziell mit Docker)</t>
+    <t>Sonntag oder Montag erledigt, Schema ist auf der phpMyAdmin online DB</t>
+  </si>
+  <si>
+    <t>Serverseitig Implementiert, Clientseitig zu 80%, noch nicht getestet</t>
+  </si>
+  <si>
+    <t>1. Navigation zwischen allen Seiten (mit redirects durch Authentif.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. Userverwaltung / Profil </t>
+  </si>
+  <si>
+    <t>3. Authentifizierung &amp; Session</t>
+  </si>
+  <si>
+    <t>4. Websockets</t>
+  </si>
+  <si>
+    <t>Chatverlauf über Mongo abspeichern und abfragen. Nicht implementiert</t>
+  </si>
+  <si>
+    <t>?????????????????????????????</t>
+  </si>
+  <si>
+    <t>Filterungssystem der Impfung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Potenziell sehr großer Aufwand durch  Berechnung anhand vom Radius (Landkreis, umliegendeLandkreise, alle) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abfragen/Erstellen/Designen von Impflisten </t>
+  </si>
+  <si>
+    <t>Abfragen/Erstellen/Designen von News</t>
+  </si>
+  <si>
+    <t>Abfragen/Erstellen/Designen von Tabellen und weiteren Elementen</t>
+  </si>
+  <si>
+    <t>Abfragen/Erstellen/Designen von Diagrammen</t>
+  </si>
+  <si>
+    <t>Detailansicht (momentane Version auf Branch nicht lauffähig)</t>
+  </si>
+  <si>
+    <t>???</t>
+  </si>
+  <si>
+    <t>Vero &amp; Maxi</t>
+  </si>
+  <si>
+    <t>Völlig unbekannter Status, totz viel arbeit ?  Risiko = MAX :D</t>
+  </si>
+  <si>
+    <t>Am besten macht jeder eine kleine, aber etwas detailierterer Auflistung von dem an was er gerade dran ist, und was wie weit ist</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="26"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="24"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="22"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -136,12 +285,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -455,145 +610,396 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0A68A5C-D9C1-4BB8-9C8C-E2E12C0DD6D5}">
-  <dimension ref="A1:E11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="79.85546875" customWidth="1"/>
     <col min="2" max="2" width="23.42578125" customWidth="1"/>
-    <col min="4" max="4" width="60.7109375" customWidth="1"/>
+    <col min="4" max="4" width="67.140625" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" t="s">
-        <v>14</v>
-      </c>
       <c r="E1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
+      <c r="B2" t="s">
+        <v>55</v>
+      </c>
       <c r="E2">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E3">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="E4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
       <c r="E5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="33.75" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" s="5">
+        <v>9999</v>
+      </c>
+      <c r="F6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="1">
-        <v>1</v>
-      </c>
-      <c r="D7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
       <c r="B8" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="1">
-        <v>0.6</v>
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
+        <v>29</v>
       </c>
       <c r="D9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C10" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A15" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0</v>
+      </c>
+      <c r="D15" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" s="6">
+        <v>9998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="4">
+        <v>1</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23" s="1">
+        <v>1</v>
+      </c>
+      <c r="D23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="D28" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>23</v>
+      </c>
+      <c r="B29" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" s="1">
+        <v>1</v>
+      </c>
+      <c r="D29" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>24</v>
+      </c>
+      <c r="B30" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>18</v>
+      </c>
+      <c r="B33" t="s">
+        <v>13</v>
+      </c>
+      <c r="C33" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="D33" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>19</v>
+      </c>
+      <c r="B34" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34" s="1">
+        <v>0</v>
+      </c>
+      <c r="D34" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>20</v>
+      </c>
+      <c r="B35" t="s">
+        <v>13</v>
+      </c>
+      <c r="C35" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>30</v>
+      </c>
+      <c r="B36" t="s">
+        <v>13</v>
+      </c>
+      <c r="C36" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="D36" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
deleted old docker configurations and updated aufgabenbereiche
</commit_message>
<xml_diff>
--- a/Aufgabenbereiche.xlsx
+++ b/Aufgabenbereiche.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael Ulrich\IBS_SS21\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C98D20DB-2FE1-4618-A911-979FB2193AC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DB7CD31-EA56-4AA0-B862-C0AFFA3B06ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
   <si>
     <t>Aufgaben:</t>
   </si>
@@ -125,14 +125,20 @@
     <t>Client muss noch Subben und reagieren</t>
   </si>
   <si>
-    <t>nodeexpressapi fehlt</t>
+    <t>Noch zu erledigen</t>
+  </si>
+  <si>
+    <t>#Alle sicherheitsrelevanten daten in .env speichern
+#Code umstrukturieren falls nötig
+#Ordnerstruktur überlegen 
+#Einloggdaten bei MongoDB aktivieren-&gt;entsprechend db config anpassen</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -162,14 +168,6 @@
       <u/>
       <sz val="24"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF0070C0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -215,7 +213,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -228,7 +225,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -236,6 +233,7 @@
     <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -553,14 +551,14 @@
   <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="79.85546875" customWidth="1"/>
-    <col min="2" max="2" width="23.42578125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" style="6"/>
+    <col min="2" max="2" width="23.42578125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" style="5"/>
     <col min="4" max="4" width="67.140625" customWidth="1"/>
     <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -569,10 +567,10 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D1" t="s">
@@ -586,10 +584,10 @@
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="6">
         <v>0.9</v>
       </c>
       <c r="D2" t="s">
@@ -603,10 +601,10 @@
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="6">
         <v>0.75</v>
       </c>
       <c r="D3" t="s">
@@ -620,10 +618,10 @@
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="6">
         <v>0.8</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -634,102 +632,99 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="13">
+      <c r="C5" s="12">
         <v>1</v>
       </c>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
     </row>
     <row r="6" spans="1:5" ht="33.75" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="6">
         <v>0.9</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="9" t="s">
         <v>31</v>
       </c>
       <c r="E6" s="3"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="13">
+      <c r="C7" s="12">
         <v>1</v>
       </c>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="6" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="13">
+      <c r="C9" s="12">
         <v>1</v>
       </c>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="13">
+      <c r="C10" s="12">
         <v>1</v>
       </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="7">
-        <v>0.75</v>
-      </c>
-      <c r="D11" t="s">
-        <v>32</v>
+      <c r="C11" s="6">
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="6">
         <v>0</v>
       </c>
     </row>
@@ -737,10 +732,10 @@
       <c r="A13" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="6">
         <v>0</v>
       </c>
     </row>
@@ -748,10 +743,10 @@
       <c r="A14" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="6">
         <v>0</v>
       </c>
     </row>
@@ -759,10 +754,10 @@
       <c r="A15" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C15" s="6">
         <v>0</v>
       </c>
       <c r="D15" t="s">
@@ -776,66 +771,71 @@
       <c r="A16" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="7">
+      <c r="C16" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
+    <row r="18" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="20" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="9"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="8"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C22" s="7"/>
+      <c r="C22" s="6"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C23" s="7"/>
+      <c r="C23" s="6"/>
     </row>
     <row r="25" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
     </row>
     <row r="27" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C28" s="7"/>
+      <c r="C28" s="6"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C29" s="7"/>
+      <c r="C29" s="6"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C30" s="7"/>
+      <c r="C30" s="6"/>
     </row>
     <row r="32" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="8"/>
-      <c r="C32" s="9"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="8"/>
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C33" s="7"/>
+      <c r="C33" s="6"/>
     </row>
     <row r="34" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C34" s="7"/>
+      <c r="C34" s="6"/>
     </row>
     <row r="35" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C35" s="7"/>
+      <c r="C35" s="6"/>
     </row>
     <row r="36" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C36" s="7"/>
+      <c r="C36" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added enviroment variables and updated aufgabenbereiche
</commit_message>
<xml_diff>
--- a/Aufgabenbereiche.xlsx
+++ b/Aufgabenbereiche.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simon Ruttmann\Desktop\InternetbasierteSystemeProjekt\IBS_SS21\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael Ulrich\IBS_SS21\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57E94878-E5E1-41E0-B089-F0369EBD8763}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="41">
   <si>
     <t>Fortschritt</t>
   </si>
@@ -47,24 +48,15 @@
     <t>Express API:</t>
   </si>
   <si>
-    <t>data-Routes</t>
-  </si>
-  <si>
     <t>user-Routes</t>
   </si>
   <si>
-    <t>auth,redirect-Routes</t>
-  </si>
-  <si>
     <t>Userverwaltung (insert, update, select)</t>
   </si>
   <si>
     <t>Authentifikation &amp; Session</t>
   </si>
   <si>
-    <t>index</t>
-  </si>
-  <si>
     <t>login</t>
   </si>
   <si>
@@ -92,21 +84,12 @@
     <t>coronaChat</t>
   </si>
   <si>
-    <t>Clientside:</t>
-  </si>
-  <si>
     <t>Macht:</t>
   </si>
   <si>
     <t>Macht</t>
   </si>
   <si>
-    <t>empty Template</t>
-  </si>
-  <si>
-    <t>empty Template, Karte erstellt</t>
-  </si>
-  <si>
     <t>done</t>
   </si>
   <si>
@@ -119,9 +102,6 @@
     <t>Daten Collect:</t>
   </si>
   <si>
-    <t>Aufbereitung muss in Logik portiert werden</t>
-  </si>
-  <si>
     <t>Server-feature</t>
   </si>
   <si>
@@ -138,12 +118,45 @@
   </si>
   <si>
     <t>Websocketbackend</t>
+  </si>
+  <si>
+    <t>Aufbereitung muss in Logik portiert werden (Datenaufbereitung nodeexpressapi -&gt;nodecollect)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data-Routes </t>
+  </si>
+  <si>
+    <t>index(Startseite)</t>
+  </si>
+  <si>
+    <t>Clientside(HTML-Seiten):</t>
+  </si>
+  <si>
+    <t>#Karte optisch fertig-&gt;integration fehlt</t>
+  </si>
+  <si>
+    <t>Keine</t>
+  </si>
+  <si>
+    <t>#Karte optisch fertig-&gt;integration fehlt
+#Weitere Datenaufbereitung fehlt</t>
+  </si>
+  <si>
+    <t>Nach Gespräch mit Prof</t>
+  </si>
+  <si>
+    <t>#Code umstrukturieren falls nötig
+#Ordnerstruktur überlegen 
+#Einloggdaten bei MongoDB aktivieren-&gt;entsprechend db config anpassen</t>
+  </si>
+  <si>
+    <t>auth, redirect-Routes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -198,7 +211,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -218,6 +231,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -267,7 +286,7 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -293,9 +312,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="2"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -305,6 +321,20 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="3"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Ausgabe" xfId="2" builtinId="21"/>
@@ -622,41 +652,44 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="79.85546875" customWidth="1"/>
-    <col min="2" max="2" width="28.85546875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="82.28515625" customWidth="1"/>
+    <col min="2" max="2" width="49.5703125" style="2" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" style="2" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
     <col min="5" max="5" width="26.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="B1" s="15" t="s">
+      <c r="A1" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="14" t="s">
-        <v>24</v>
+      <c r="D1" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="15" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="4"/>
@@ -666,7 +699,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" t="s">
@@ -675,66 +708,66 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="D5" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="11">
+        <v>1</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="11">
+        <v>1</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="3">
-        <v>1</v>
-      </c>
-      <c r="D6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B8" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="11">
+        <v>1</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="3">
-        <v>1</v>
-      </c>
-      <c r="D7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="5">
-        <v>1</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="3">
-        <v>1</v>
-      </c>
-      <c r="D9" s="7" t="s">
+      <c r="B9" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="11">
+        <v>1</v>
+      </c>
+      <c r="D9" s="9" t="s">
         <v>4</v>
       </c>
       <c r="E9" s="1"/>
@@ -746,195 +779,213 @@
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="11">
+        <v>1</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="7"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="20">
+        <v>0.75</v>
+      </c>
+      <c r="D14" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="11">
+        <v>1</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A17" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="22" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" s="1" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="17" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>37</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="3">
-        <v>1</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" s="7"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>34</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" s="3">
-        <v>1</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E14" s="1"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" s="3">
-        <v>1</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="B19" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="D19" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="E19" s="14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" s="1" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>26</v>
+      <c r="B20" s="22" t="s">
+        <v>35</v>
       </c>
       <c r="C20" s="3">
         <v>0.2</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E20"/>
+      <c r="E20" s="2" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="21" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="18" t="s">
-        <v>13</v>
+      <c r="A21" s="17" t="s">
+        <v>10</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C21" s="11">
         <v>1</v>
       </c>
-      <c r="D21" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="E21" s="9" t="s">
-        <v>27</v>
+      <c r="D21" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="18" t="s">
-        <v>14</v>
+      <c r="A22" s="17" t="s">
+        <v>11</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C22" s="11">
         <v>1</v>
       </c>
-      <c r="D22" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="E22" s="9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>26</v>
+      <c r="D22" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" s="22" t="s">
+        <v>37</v>
       </c>
       <c r="C23" s="3">
         <v>0.2</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="E23" s="2" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="24" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="18" t="s">
-        <v>16</v>
+      <c r="A24" s="17" t="s">
+        <v>13</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C24" s="3">
         <v>0.6</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="E24" s="2"/>
     </row>
     <row r="25" spans="1:5" s="1" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="18" t="s">
-        <v>17</v>
+      <c r="A25" s="17" t="s">
+        <v>14</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C25" s="11">
         <v>1</v>
       </c>
-      <c r="D25" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="E25" s="9" t="s">
-        <v>27</v>
+      <c r="D25" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="18" t="s">
-        <v>18</v>
+      <c r="A26" s="17" t="s">
+        <v>15</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="C26" s="3">
         <v>0.2</v>
       </c>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="27" spans="1:5" s="1" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="18" t="s">
-        <v>21</v>
+      <c r="A27" s="17" t="s">
+        <v>18</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C27" s="12">
-        <v>1</v>
-      </c>
-      <c r="D27" t="s">
-        <v>4</v>
-      </c>
-      <c r="E27" t="s">
-        <v>29</v>
+        <v>21</v>
+      </c>
+      <c r="C27" s="11">
+        <v>1</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -950,7 +1001,7 @@
         <v>0</v>
       </c>
       <c r="G37" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="38" spans="6:7" x14ac:dyDescent="0.25">

</xml_diff>